<commit_message>
Added flags to operon events
These flag track whether the operons were reversed or not
</commit_message>
<xml_diff>
--- a/excel_files/Comparison - Ancestor 1 & NC_016023.xlsx
+++ b/excel_files/Comparison - Ancestor 1 & NC_016023.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="73">
   <si>
     <t>Ancestor 1</t>
   </si>
@@ -23,55 +23,55 @@
     <t>NC_016023</t>
   </si>
   <si>
-    <t>[16S, 23S,5S]</t>
-  </si>
-  <si>
-    <t>[ , V,a,l,_,G,U,C]</t>
-  </si>
-  <si>
-    <t>[ , -,S,e,c,_,U,G,A]</t>
-  </si>
-  <si>
-    <t>[ , A,l,a,_,G,C,C]</t>
-  </si>
-  <si>
-    <t>[ , -,A,r,g,_,C,G,A]</t>
-  </si>
-  <si>
-    <t>[Met_AUG, Met_AUG,Ser_UCA]</t>
-  </si>
-  <si>
-    <t>[16S, Ile_AUC,Ala_GCA,23S,5S,Val_GUA,Thr_ACA,Lys_AAA,Leu_CUG,Gly_GGC,Leu_UUA,Arg_CGU,Pro_CCA,Ala_GCA,16S,23S,5S]</t>
-  </si>
-  <si>
-    <t>[Thr_ACA, Phe_UUC,Asp_GAC,Met_AUG,Glu_GAA]</t>
-  </si>
-  <si>
-    <t>[16S, 23S,5S,Ala_GCA,Met_AUG,Ser_UCA,Asp_GAC,Tyr_UAC,Trp_UGG,His_CAC,Gln_CAA,Gly_GGC,Arg_CGU,Gly_GGA,Ile_AUC,Asn_AAC,Glu_GAA,Lys_AAA]</t>
-  </si>
-  <si>
-    <t>[Asn_AAC, Ser_AGC,Glu_GAA,Val_GUA,Asp_GAC,Leu_CUA,Leu_CUC,Pro_CCA,Gly_GGA,Ile_AUC,16S,23S,5S]</t>
-  </si>
-  <si>
-    <t>[16S, 23S,5S,Asn_AAC,Ser_UCC,Glu_GAA,Val_GUA,Met_AUG,Asp_GAC,Phe_UUC,Thr_ACA,Tyr_UAC,His_CAC,Gln_CAA,Gly_GGC,Cys_UGC,Leu_UUA,Leu_UUG]</t>
-  </si>
-  <si>
-    <t>[ , -,A,r,g,_,A,G,G]</t>
-  </si>
-  <si>
-    <t>[ , A,r,g,_,A,G,A]</t>
-  </si>
-  <si>
-    <t>[ , -,T,r,p,_,N,N,N]</t>
-  </si>
-  <si>
-    <t>[[, 5,S,,, ,A,s,n,_,A,A,C,,, ,T,h,r,_,A,C,C,,, ,G,l,u,_,G,A,A,,, ,G,l,n,_,C,A,A,]]</t>
-  </si>
-  <si>
-    <t>[[, A,s,n,_,A,A,C,,, ,A,s,n,_,A,A,C,,, ,A,s,n,_,A,A,C,,, ,T,h,r,_,A,C,C,,, ,G,l,u,_,G,A,A,,, ,G,l,n,_,C,A,A,,, ,L,y,s,_,A,A,A,,, ,A,l,a,_,G,C,A,]]</t>
-  </si>
-  <si>
-    <t>[-, [,A,r,g,_,A,G,A,,, ,G,l,y,_,G,G,A,]]</t>
+    <t>[16S, 23S, 5S]</t>
+  </si>
+  <si>
+    <t>[ Val_GUC]</t>
+  </si>
+  <si>
+    <t>[ -Sec_UGA]</t>
+  </si>
+  <si>
+    <t>[ Ala_GCC]</t>
+  </si>
+  <si>
+    <t>[ -Arg_CGA]</t>
+  </si>
+  <si>
+    <t>[Met_AUG, Met_AUG, Ser_UCA]</t>
+  </si>
+  <si>
+    <t>[16S, Ile_AUC, Ala_GCA, 23S, 5S, Val_GUA, Thr_ACA, Lys_AAA, Leu_CUG, Gly_GGC, Leu_UUA, Arg_CGU, Pro_CCA, Ala_GCA, 16S, 23S, 5S]</t>
+  </si>
+  <si>
+    <t>[Thr_ACA, Phe_UUC, Asp_GAC, Met_AUG, Glu_GAA]</t>
+  </si>
+  <si>
+    <t>[16S, 23S, 5S, Ala_GCA, Met_AUG, Ser_UCA, Asp_GAC, Tyr_UAC, Trp_UGG, His_CAC, Gln_CAA, Gly_GGC, Arg_CGU, Gly_GGA, Ile_AUC, Asn_AAC, Glu_GAA, Lys_AAA]</t>
+  </si>
+  <si>
+    <t>[Asn_AAC, Ser_AGC, Glu_GAA, Val_GUA, Asp_GAC, Leu_CUA, Leu_CUC, Pro_CCA, Gly_GGA, Ile_AUC, 16S, 23S, 5S]</t>
+  </si>
+  <si>
+    <t>[16S, 23S, 5S, Asn_AAC, Ser_UCC, Glu_GAA, Val_GUA, Met_AUG, Asp_GAC, Phe_UUC, Thr_ACA, Tyr_UAC, His_CAC, Gln_CAA, Gly_GGC, Cys_UGC, Leu_UUA, Leu_UUG]</t>
+  </si>
+  <si>
+    <t>[ -Arg_AGG]</t>
+  </si>
+  <si>
+    <t>[ Arg_AGA]</t>
+  </si>
+  <si>
+    <t>[ -Trp_NNN]</t>
+  </si>
+  <si>
+    <t>[5S, Asn_AAC, Thr_ACC, Glu_GAA, Gln_CAA]</t>
+  </si>
+  <si>
+    <t>[Asn_AAC, Asn_AAC, Asn_AAC, Thr_ACC, Glu_GAA, Gln_CAA, Lys_AAA, Ala_GCA]</t>
+  </si>
+  <si>
+    <t>-[Arg_AGA, Gly_GGA]</t>
   </si>
   <si>
     <t xml:space="preserve"> Asp_GAC</t>
@@ -83,9 +83,6 @@
     <t>[Asn_AAC, Ser_AGC, Glu_GAA, Asp_GAC, Gln_CAA, Lys_AAA, Leu_CUA, Gly_GGC, Leu_CUC, Arg_CGU, Pro_CCA, Gly_GGA, 16S, 23S, 5S, Met_AUG]</t>
   </si>
   <si>
-    <t>[16S, 23S, 5S]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -Arg_AGG</t>
   </si>
   <si>
@@ -173,70 +170,70 @@
     <t>10.0</t>
   </si>
   <si>
+    <t>0*</t>
+  </si>
+  <si>
     <t>16.0</t>
   </si>
   <si>
+    <t>17.0</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>16.5</t>
+  </si>
+  <si>
+    <t>13.5</t>
+  </si>
+  <si>
+    <t>4.0*</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>17.5</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>18.0</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>2.0*</t>
+  </si>
+  <si>
     <t>8.0</t>
   </si>
   <si>
-    <t>18.0</t>
-  </si>
-  <si>
-    <t>23.0</t>
-  </si>
-  <si>
-    <t>12.0</t>
-  </si>
-  <si>
-    <t>17.0</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>14.0</t>
-  </si>
-  <si>
-    <t>16.5</t>
-  </si>
-  <si>
-    <t>13.5</t>
-  </si>
-  <si>
-    <t>4.0*</t>
-  </si>
-  <si>
-    <t>21.0</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>11.0</t>
-  </si>
-  <si>
-    <t>17.5</t>
-  </si>
-  <si>
-    <t>7.0</t>
-  </si>
-  <si>
-    <t>12.5</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>2.0*</t>
-  </si>
-  <si>
-    <t>44.0</t>
-  </si>
-  <si>
-    <t>79.0</t>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>22.0</t>
   </si>
 </sst>
 </file>
@@ -597,67 +594,67 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>29</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>33</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>34</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>36</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>37</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>38</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>39</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" t="s">
-        <v>41</v>
-      </c>
       <c r="Z2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -665,76 +662,76 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
         <v>45</v>
       </c>
-      <c r="I3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="s">
         <v>46</v>
       </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3" t="s">
         <v>48</v>
       </c>
-      <c r="Q3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" t="s">
-        <v>46</v>
-      </c>
-      <c r="T3" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>49</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" t="s">
         <v>50</v>
       </c>
-      <c r="W3" t="s">
-        <v>42</v>
-      </c>
-      <c r="X3" t="s">
-        <v>51</v>
-      </c>
       <c r="Y3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -742,76 +739,76 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
         <v>45</v>
       </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
         <v>46</v>
       </c>
-      <c r="K4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" t="s">
-        <v>42</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N4" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" t="s">
-        <v>42</v>
-      </c>
-      <c r="R4" t="s">
-        <v>42</v>
-      </c>
-      <c r="S4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T4" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>49</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" t="s">
         <v>50</v>
       </c>
-      <c r="W4" t="s">
-        <v>42</v>
-      </c>
-      <c r="X4" t="s">
-        <v>51</v>
-      </c>
       <c r="Y4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -819,76 +816,76 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="N5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P5" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="R5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="T5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U5" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="V5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="W5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -899,76 +896,76 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="N6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="Q6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="T6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U6" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="V6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="W6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -976,76 +973,76 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="N7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="Q7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="T7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U7" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="V7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="W7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1053,76 +1050,76 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M8" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="N8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="Q8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="T8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U8" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="V8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="W8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1130,76 +1127,76 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>52</v>
       </c>
       <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" t="s">
         <v>46</v>
       </c>
-      <c r="G9" t="s">
+      <c r="N9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" t="s">
+        <v>41</v>
+      </c>
+      <c r="S9" t="s">
+        <v>54</v>
+      </c>
+      <c r="T9" t="s">
+        <v>41</v>
+      </c>
+      <c r="U9" t="s">
+        <v>55</v>
+      </c>
+      <c r="V9" t="s">
+        <v>56</v>
+      </c>
+      <c r="W9" t="s">
+        <v>41</v>
+      </c>
+      <c r="X9" t="s">
         <v>42</v>
       </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" t="s">
-        <v>42</v>
-      </c>
-      <c r="O9" t="s">
-        <v>42</v>
-      </c>
-      <c r="P9" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>42</v>
-      </c>
-      <c r="R9" t="s">
-        <v>42</v>
-      </c>
-      <c r="S9" t="s">
-        <v>58</v>
-      </c>
-      <c r="T9" t="s">
-        <v>42</v>
-      </c>
-      <c r="U9" t="s">
+      <c r="Y9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" t="s">
         <v>56</v>
-      </c>
-      <c r="V9" t="s">
-        <v>59</v>
-      </c>
-      <c r="W9" t="s">
-        <v>42</v>
-      </c>
-      <c r="X9" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -1207,76 +1204,76 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
         <v>52</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" t="s">
         <v>52</v>
       </c>
       <c r="K10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M10" t="s">
         <v>52</v>
       </c>
       <c r="N10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="T10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Y10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -1284,76 +1281,76 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" t="s">
+        <v>41</v>
+      </c>
+      <c r="P11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R11" t="s">
+        <v>41</v>
+      </c>
+      <c r="S11" t="s">
+        <v>62</v>
+      </c>
+      <c r="T11" t="s">
+        <v>41</v>
+      </c>
+      <c r="U11" t="s">
+        <v>63</v>
+      </c>
+      <c r="V11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W11" t="s">
+        <v>41</v>
+      </c>
+      <c r="X11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M11" t="s">
-        <v>64</v>
-      </c>
-      <c r="N11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>42</v>
-      </c>
-      <c r="R11" t="s">
-        <v>42</v>
-      </c>
-      <c r="S11" t="s">
-        <v>65</v>
-      </c>
-      <c r="T11" t="s">
-        <v>42</v>
-      </c>
-      <c r="U11" t="s">
-        <v>66</v>
-      </c>
-      <c r="V11" t="s">
-        <v>59</v>
-      </c>
-      <c r="W11" t="s">
-        <v>42</v>
-      </c>
-      <c r="X11" t="s">
-        <v>43</v>
-      </c>
       <c r="Y11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -1361,73 +1358,73 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
         <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
         <v>42</v>
       </c>
-      <c r="H12" t="s">
-        <v>43</v>
-      </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M12" t="s">
         <v>52</v>
       </c>
       <c r="N12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P12" t="s">
         <v>52</v>
       </c>
       <c r="Q12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="T12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="V12" t="s">
         <v>52</v>
       </c>
       <c r="W12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Y12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z12" t="s">
         <v>52</v>
@@ -1438,76 +1435,76 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="K13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O13" t="s">
+        <v>41</v>
+      </c>
+      <c r="P13" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>41</v>
+      </c>
+      <c r="R13" t="s">
+        <v>41</v>
+      </c>
+      <c r="S13" t="s">
+        <v>67</v>
+      </c>
+      <c r="T13" t="s">
+        <v>41</v>
+      </c>
+      <c r="U13" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13" t="s">
+        <v>50</v>
+      </c>
+      <c r="W13" t="s">
+        <v>41</v>
+      </c>
+      <c r="X13" t="s">
         <v>68</v>
       </c>
-      <c r="F13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" t="s">
-        <v>42</v>
-      </c>
-      <c r="M13" t="s">
-        <v>54</v>
-      </c>
-      <c r="N13" t="s">
-        <v>42</v>
-      </c>
-      <c r="O13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P13" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>42</v>
-      </c>
-      <c r="R13" t="s">
-        <v>42</v>
-      </c>
-      <c r="S13" t="s">
-        <v>69</v>
-      </c>
-      <c r="T13" t="s">
-        <v>42</v>
-      </c>
-      <c r="U13" t="s">
-        <v>69</v>
-      </c>
-      <c r="V13" t="s">
-        <v>51</v>
-      </c>
-      <c r="W13" t="s">
-        <v>42</v>
-      </c>
-      <c r="X13" t="s">
-        <v>70</v>
-      </c>
       <c r="Y13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -1515,76 +1512,76 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
         <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J14" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="K14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M14" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="N14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P14" t="s">
         <v>52</v>
       </c>
       <c r="Q14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="T14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V14" t="s">
+        <v>53</v>
+      </c>
+      <c r="W14" t="s">
+        <v>41</v>
+      </c>
+      <c r="X14" t="s">
         <v>57</v>
       </c>
-      <c r="W14" t="s">
-        <v>42</v>
-      </c>
-      <c r="X14" t="s">
-        <v>60</v>
-      </c>
       <c r="Y14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -1592,76 +1589,76 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="H15" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J15" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M15" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="N15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P15" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="Q15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S15" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="T15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U15" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="V15" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="W15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z15" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -1669,76 +1666,76 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="K16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M16" t="s">
-        <v>55</v>
-      </c>
-      <c r="N16" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="O16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P16" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="Q16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S16" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="T16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U16" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="V16" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="W16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z16" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:26">
@@ -1746,76 +1743,76 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="I17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J17" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M17" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="N17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P17" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="Q17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S17" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="T17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U17" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="V17" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="W17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z17" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:26">
@@ -1823,76 +1820,76 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H18" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J18" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="K18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M18" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="N18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P18" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="Q18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S18" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="T18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U18" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="V18" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="W18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X18" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="Y18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z18" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:26">
@@ -1900,76 +1897,76 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H19" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="I19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U19" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="V19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="W19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X19" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="Y19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="2:26">
@@ -1977,76 +1974,76 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H20" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="I20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M20" t="s">
+        <v>72</v>
+      </c>
+      <c r="N20" t="s">
+        <v>41</v>
+      </c>
+      <c r="O20" t="s">
+        <v>41</v>
+      </c>
+      <c r="P20" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>41</v>
+      </c>
+      <c r="R20" t="s">
+        <v>41</v>
+      </c>
+      <c r="S20" t="s">
+        <v>49</v>
+      </c>
+      <c r="T20" t="s">
+        <v>41</v>
+      </c>
+      <c r="U20" t="s">
         <v>55</v>
       </c>
-      <c r="N20" t="s">
-        <v>42</v>
-      </c>
-      <c r="O20" t="s">
-        <v>42</v>
-      </c>
-      <c r="P20" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>42</v>
-      </c>
-      <c r="R20" t="s">
-        <v>42</v>
-      </c>
-      <c r="S20" t="s">
-        <v>47</v>
-      </c>
-      <c r="T20" t="s">
-        <v>42</v>
-      </c>
-      <c r="U20" t="s">
-        <v>47</v>
-      </c>
       <c r="V20" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="W20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X20" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="Y20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z20" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2078,67 +2075,67 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>29</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>33</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>34</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>36</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>37</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>38</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>39</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" t="s">
-        <v>41</v>
-      </c>
       <c r="Z2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:26">

</xml_diff>